<commit_message>
new screan with UI
</commit_message>
<xml_diff>
--- a/gra_1/TouchGFX/assets/texts/texts.xlsx
+++ b/gra_1/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="49">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -141,6 +141,27 @@
   </si>
   <si>
     <t xml:space="preserve">Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Nowa Gra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wyjdź</t>
   </si>
 </sst>
 </file>
@@ -1601,6 +1622,40 @@
         <v>36</v>
       </c>
     </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
add menu and screen transition
</commit_message>
<xml_diff>
--- a/gra_1/TouchGFX/assets/texts/texts.xlsx
+++ b/gra_1/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="54">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -141,6 +141,42 @@
   </si>
   <si>
     <t xml:space="preserve">Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Nowa Gra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wyjdź</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comicbd.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FlaBi</t>
   </si>
 </sst>
 </file>
@@ -1471,6 +1507,25 @@
       <c r="P6" s="10"/>
     </row>
     <row r="7" spans="2:16">
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>83</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
       <c r="L7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1601,6 +1656,57 @@
         <v>36</v>
       </c>
     </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>